<commit_message>
Removing cd from lint test
</commit_message>
<xml_diff>
--- a/AutoTest_gitclassroom_tests.xlsx
+++ b/AutoTest_gitclassroom_tests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmt/Library/CloudStorage/Dropbox/UCA/Data Structures/source/LinkedList_Project/LinkedList_Project_AutoTest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michelle/Dropbox/UCA/Data Structures/source/LinkedList_Project/LinkedList_Project_AutoTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62ED7760-728E-1E4D-8EE0-8FF14AFFED83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BCEAD3-644E-A242-A392-595CC178379D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57420" yWindow="-5180" windowWidth="41400" windowHeight="16520" xr2:uid="{29F2130F-3E6E-6C43-8BD2-2E7492F933ED}"/>
+    <workbookView xWindow="840" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{29F2130F-3E6E-6C43-8BD2-2E7492F933ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Classroom" sheetId="1" r:id="rId1"/>
@@ -57,15 +57,9 @@
     <t>Points</t>
   </si>
   <si>
-    <t>git clone https://github.com/TeacherTalley/LinkedList_AutoTest.git</t>
-  </si>
-  <si>
     <t>Install test code, copy student source, build student and test code</t>
   </si>
   <si>
-    <t>cd LinkedList_AutoTest &amp;&amp; ./AutoTest_setup.sh</t>
-  </si>
-  <si>
     <t>Main Output</t>
   </si>
   <si>
@@ -75,9 +69,6 @@
     <t>Coding Style</t>
   </si>
   <si>
-    <t>./LinkedList_AutoTest/AutoTest_Style.sh</t>
-  </si>
-  <si>
     <t>Run cpplint on student code</t>
   </si>
   <si>
@@ -111,15 +102,6 @@
     <t>Verify use of std::list for removing from list</t>
   </si>
   <si>
-    <t>./LinkedList/AutoTest/AutoTest_OutputTest.py -t test_missing_file</t>
-  </si>
-  <si>
-    <t>./LinkedList/AutoTest/AutoTest_OutputTest.py -t test_main_output</t>
-  </si>
-  <si>
-    <t>./LinkedList/AutoTest/AutoTest_OutputTest.py -t test_output_file</t>
-  </si>
-  <si>
     <t>Error: Test for missing input files</t>
   </si>
   <si>
@@ -130,6 +112,24 @@
   </si>
   <si>
     <t>AutoGrading Rubric</t>
+  </si>
+  <si>
+    <t>cd LinkedList_Project_AutoTest &amp;&amp; ./AutoTest_setup.sh</t>
+  </si>
+  <si>
+    <t>./LinkedList_Project_AutoTest/AutoTest_Style.sh</t>
+  </si>
+  <si>
+    <t>./LinkedList_Project_AutoTest/AutoTest/AutoTest_OutputTest.py -t test_missing_file</t>
+  </si>
+  <si>
+    <t>./LinkedList_Project_AutoTest/AutoTest/AutoTest_OutputTest.py -t test_main_output</t>
+  </si>
+  <si>
+    <t>./LinkedList_Project_AutoTest/AutoTest/AutoTest_OutputTest.py -t test_output_file</t>
+  </si>
+  <si>
+    <t>git clone https://github.com/TeacherTalley/LinkedList_Project_AutoTest</t>
   </si>
 </sst>
 </file>
@@ -197,9 +197,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -237,7 +237,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -343,7 +343,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -485,7 +485,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -495,16 +495,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D968784-9ABC-434B-B612-3087309D1BAB}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:E14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.1640625" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="68.1640625" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="53" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -534,13 +534,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -548,13 +548,13 @@
     </row>
     <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E4">
         <v>5</v>
@@ -562,13 +562,13 @@
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>27</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -576,13 +576,13 @@
     </row>
     <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E6">
         <v>20</v>
@@ -590,13 +590,13 @@
     </row>
     <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E7">
         <v>30</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2"/>
       <c r="E8">
@@ -614,13 +614,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2"/>
       <c r="E10">
@@ -629,7 +629,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2"/>
       <c r="E11">
@@ -638,7 +638,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2"/>
       <c r="E12">
@@ -647,7 +647,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2"/>
       <c r="E13">
@@ -656,7 +656,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2"/>
       <c r="E14">
@@ -665,7 +665,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2"/>
       <c r="E15">
@@ -675,7 +675,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2"/>
       <c r="E16">
@@ -744,7 +744,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -754,7 +754,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -762,10 +762,10 @@
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -773,10 +773,10 @@
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -784,10 +784,10 @@
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>20</v>
@@ -795,10 +795,10 @@
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>30</v>
@@ -806,7 +806,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8">
@@ -816,13 +816,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10">
@@ -831,7 +831,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11">
@@ -840,7 +840,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12">
@@ -849,7 +849,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13">
@@ -858,7 +858,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14">
@@ -867,7 +867,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15">
@@ -877,7 +877,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C16">
         <f>C8+C15</f>

</xml_diff>

<commit_message>
Update points for project
</commit_message>
<xml_diff>
--- a/AutoTest_gitclassroom_tests.xlsx
+++ b/AutoTest_gitclassroom_tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmt/Library/CloudStorage/Dropbox/UCA/Data Structures/source/LinkedList_Project/LinkedList_Project_AutoTest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michelle/Dropbox/UCA/Data Structures/source/LinkedList_Project/LinkedList_Project_AutoTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B8E42B-238B-EF4D-89B8-44042903A1CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE748928-F7CB-324D-B1E4-879AD7532E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30860" yWindow="-7120" windowWidth="28800" windowHeight="16520" activeTab="1" xr2:uid="{29F2130F-3E6E-6C43-8BD2-2E7492F933ED}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{29F2130F-3E6E-6C43-8BD2-2E7492F933ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Classroom" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>AutoTest Setup</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>Close all files after use (read and write)</t>
-  </si>
-  <si>
-    <t>AutoGrading Rubric</t>
   </si>
   <si>
     <t>cd LinkedList_Project_AutoTest &amp;&amp; ./AutoTest_setup.sh</t>
@@ -549,10 +546,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -566,7 +563,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4">
         <v>5</v>
@@ -580,7 +577,7 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -594,7 +591,7 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6">
         <v>20</v>
@@ -608,7 +605,7 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7">
         <v>30</v>
@@ -730,10 +727,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B4171E-9FB2-AA44-B865-923DD5DD382A}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -754,63 +751,67 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C7">
         <v>20</v>
@@ -818,105 +819,49 @@
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>34</v>
-      </c>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2"/>
       <c r="C9">
-        <v>20</v>
+        <f>SUM(C2:C8)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
+      <c r="A10" s="1"/>
       <c r="B10" s="2"/>
-      <c r="C10">
-        <f>SUM(C3:C9)</f>
-        <v>100</v>
-      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
       <c r="B12" s="2"/>
-      <c r="C12">
-        <v>10</v>
-      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
       <c r="B13" s="2"/>
-      <c r="C13">
-        <v>10</v>
-      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
       <c r="B14" s="2"/>
-      <c r="C14">
-        <v>10</v>
-      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
       <c r="B15" s="2"/>
-      <c r="C15">
-        <v>3</v>
-      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
       <c r="B16" s="2"/>
-      <c r="C16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17">
-        <f>SUM(C12:C16)</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18">
-        <f>C10+C17</f>
-        <v>135</v>
-      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>